<commit_message>
Solved 2 pratice problems
</commit_message>
<xml_diff>
--- a/algorithms&data/python-labs/lab6/auto_report/reports/currency_report.xlsx
+++ b/algorithms&data/python-labs/lab6/auto_report/reports/currency_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,6 +547,27 @@
         <v>82.203</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-09 01:24:12</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.8569</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3.2454</v>
+      </c>
+      <c r="E7" t="n">
+        <v>82.203</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>